<commit_message>
Add and update test case and scenario spreadsheets
Added new TestCases.xls and TestCases.xlsx files to the TestCases directory. Updated the TestScenarios.xlsx file in the TestScenarios directory with new changes.
</commit_message>
<xml_diff>
--- a/SauceDemo/TestScenarios/TestScenarios.xlsx
+++ b/SauceDemo/TestScenarios/TestScenarios.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\QA-Portolio\SauceDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\QA-Portolio\SauceDemo\TestScenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBE6E156-80F5-4F19-ADD3-B7026681956B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B51FD8CC-223B-4314-B591-31B7B901B58F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5088" xr2:uid="{40CE6357-F45D-4EBE-BCF1-4688B14FF024}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -70,14 +70,67 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Split into multiple negative cases</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>SC006</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>SC007</t>
+  </si>
+  <si>
+    <t>SC008</t>
+  </si>
+  <si>
+    <t>SC009</t>
+  </si>
+  <si>
+    <t>User sorts products in inventory page</t>
+  </si>
+  <si>
+    <t>Split into multiple type of sort methods</t>
+  </si>
+  <si>
+    <t>User removes products from cart</t>
+  </si>
+  <si>
+    <t>User resets application state from menu</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>User goes to about section from menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,13 +158,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -122,6 +195,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E777937E-94E3-4973-B3DB-61BBF2EF5559}" name="Tabela1" displayName="Tabela1" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E1048576" xr:uid="{F4AE6884-74B1-43EC-ACE7-FD5F1B5C9B05}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{DD7BA6D6-82B9-46D7-86BE-03C2414F4F9C}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{E262A6C7-7806-45F9-AD6C-8C3329BE6AE5}" name="Scenario"/>
+    <tableColumn id="3" xr3:uid="{3A66DDD7-224B-44B7-BEE5-EA63A20FB3BF}" name="Priority"/>
+    <tableColumn id="4" xr3:uid="{3919D18A-584B-4405-9BBB-7A8DDEF8D06F}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{7747EFB0-AF8D-4A67-8697-728FDC419347}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,29 +514,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F632F795-4812-4967-88B8-3C2E367A1711}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="49.109375" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -453,8 +554,11 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -464,8 +568,14 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -475,8 +585,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -486,8 +599,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -497,8 +613,82 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{ED618A30-133D-410A-B1A5-54C1BB4D2AA7}">
+      <formula1>"Low, Medium, High"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D9290618-1608-4EE4-A191-A2450FCDEBF4}">
+      <formula1>"To Do, Done, Failed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>